<commit_message>
Updates and fixes to parser. Some bugs remain
</commit_message>
<xml_diff>
--- a/data/StudentResults.xlsx
+++ b/data/StudentResults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jefferyyang/Documents/GitHub.nosync/pointers/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18DC57C-95A0-EE47-AEE4-664BF4467056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27EB033-2CE3-9147-ADB7-25A06163C6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A3A07051-2C53-5D42-A22A-1C950ED41CC2}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="total2a">Sheet1!$B$22:$B$40:'Sheet1'!$B$2:$B$21</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Timeout on 6</t>
   </si>
@@ -108,13 +108,19 @@
   </si>
   <si>
     <t>Question 2b</t>
+  </si>
+  <si>
+    <t>2b score somewhat unclear</t>
+  </si>
+  <si>
+    <t>Per. Question Pts. Lost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,6 +147,13 @@
     <font>
       <b/>
       <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -177,8 +190,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -186,12 +200,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -503,13 +518,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C276C6-7B64-EC4B-B4F7-79A343B3EE85}">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,7 +536,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -551,6 +566,9 @@
         <v>0</v>
       </c>
       <c r="B2">
+        <v>-0.5</v>
+      </c>
+      <c r="C2">
         <v>-0.5</v>
       </c>
       <c r="D2">
@@ -574,6 +592,9 @@
       <c r="B3">
         <v>0</v>
       </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
       <c r="D3">
         <v>0</v>
       </c>
@@ -592,6 +613,9 @@
       <c r="B4">
         <v>0</v>
       </c>
+      <c r="C4">
+        <v>-0.5</v>
+      </c>
       <c r="D4">
         <v>0</v>
       </c>
@@ -610,6 +634,9 @@
       <c r="B5">
         <v>0</v>
       </c>
+      <c r="C5">
+        <v>-3</v>
+      </c>
       <c r="D5">
         <v>-1</v>
       </c>
@@ -628,6 +655,9 @@
       <c r="B6">
         <v>0</v>
       </c>
+      <c r="C6">
+        <v>-3</v>
+      </c>
       <c r="D6">
         <v>0</v>
       </c>
@@ -646,6 +676,9 @@
       <c r="B7">
         <v>0</v>
       </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
       <c r="D7">
         <v>0</v>
       </c>
@@ -664,6 +697,9 @@
       <c r="B8">
         <v>0</v>
       </c>
+      <c r="C8">
+        <v>-0.5</v>
+      </c>
       <c r="D8">
         <v>0</v>
       </c>
@@ -682,6 +718,9 @@
       <c r="B9">
         <v>0</v>
       </c>
+      <c r="C9">
+        <v>-1.5</v>
+      </c>
       <c r="D9">
         <v>0</v>
       </c>
@@ -700,6 +739,9 @@
       <c r="B10">
         <v>0</v>
       </c>
+      <c r="C10">
+        <v>-0.5</v>
+      </c>
       <c r="D10">
         <v>0</v>
       </c>
@@ -718,6 +760,9 @@
       <c r="B11">
         <v>0</v>
       </c>
+      <c r="C11">
+        <v>-2</v>
+      </c>
       <c r="D11">
         <v>0</v>
       </c>
@@ -736,6 +781,9 @@
       <c r="B12">
         <v>-0.5</v>
       </c>
+      <c r="C12">
+        <v>-3</v>
+      </c>
       <c r="D12">
         <v>0</v>
       </c>
@@ -754,6 +802,9 @@
       <c r="B13">
         <v>0</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
       <c r="D13">
         <v>0</v>
       </c>
@@ -772,6 +823,9 @@
       <c r="B14">
         <v>0</v>
       </c>
+      <c r="C14">
+        <v>-2</v>
+      </c>
       <c r="D14">
         <v>0</v>
       </c>
@@ -793,6 +847,9 @@
       <c r="B15">
         <v>0</v>
       </c>
+      <c r="C15">
+        <v>-0.5</v>
+      </c>
       <c r="D15">
         <v>0</v>
       </c>
@@ -811,6 +868,9 @@
       <c r="B16">
         <v>0</v>
       </c>
+      <c r="C16">
+        <v>-2</v>
+      </c>
       <c r="D16">
         <v>0</v>
       </c>
@@ -821,13 +881,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B17">
         <v>0</v>
+      </c>
+      <c r="C17">
+        <v>-0.5</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -842,7 +905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -850,6 +913,9 @@
       <c r="B18">
         <v>0</v>
       </c>
+      <c r="C18">
+        <v>-3</v>
+      </c>
       <c r="D18">
         <v>0</v>
       </c>
@@ -859,7 +925,7 @@
       <c r="F18" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J18">
@@ -867,24 +933,31 @@
         <v>3</v>
       </c>
       <c r="K18">
+        <f>COUNTIF(C2:C21,"&lt;&gt;0")</f>
+        <v>18</v>
+      </c>
+      <c r="L18">
         <f>COUNTIF(D2:D21,"&lt;&gt;0")</f>
         <v>3</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <f>COUNTIF(E2:E21,"&lt;&gt;0")</f>
         <v>10</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <f>COUNTIFS(E2:E21,"&lt;&gt;0",F2:F21,"FALSE")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
@@ -896,7 +969,7 @@
       <c r="F19" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J19">
@@ -904,25 +977,32 @@
         <v>-1.5</v>
       </c>
       <c r="K19">
+        <f>SUM(C2:C21)</f>
+        <v>-28</v>
+      </c>
+      <c r="L19">
         <f>SUM(D2:D21)</f>
         <v>-2</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <f>SUM(E2:E21)</f>
         <v>-43</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <f>SUMIF(F2:F21,"FALSE",E2:E21)</f>
         <v>-17</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B20">
         <v>-0.5</v>
+      </c>
+      <c r="C20">
+        <v>-3</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -936,7 +1016,7 @@
       <c r="G20" t="s">
         <v>4</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J20">
@@ -944,19 +1024,23 @@
         <v>-7.4999999999999997E-2</v>
       </c>
       <c r="K20">
+        <f>AVERAGE(C2:C21)</f>
+        <v>-1.4</v>
+      </c>
+      <c r="L20">
         <f>AVERAGE(D2:D21)</f>
         <v>-0.1</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <f>AVERAGE(E2:E21)</f>
         <v>-2.15</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <f>AVERAGEIF(F2:F21,"FALSE",E2:E21)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -964,6 +1048,9 @@
       <c r="B21">
         <v>0</v>
       </c>
+      <c r="C21">
+        <v>-0.5</v>
+      </c>
       <c r="D21">
         <v>0</v>
       </c>
@@ -973,7 +1060,7 @@
       <c r="F21" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J21">
@@ -981,25 +1068,32 @@
         <v>-0.5</v>
       </c>
       <c r="K21">
+        <f>AVERAGEIF(C2:C21,"&lt;&gt;0")</f>
+        <v>-1.5555555555555556</v>
+      </c>
+      <c r="L21">
         <f>AVERAGEIF(D2:D21,"&lt;&gt;0")</f>
         <v>-0.66666666666666663</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <f>AVERAGEIF(E2:E21,"&lt;&gt;0")</f>
         <v>-4.3</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <f>AVERAGEIFS(E2:E21,E2:E21,"&lt;&gt;0",F2:F21,"FALSE")</f>
         <v>-2.4285714285714284</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
         <v>0</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
       <c r="D22">
         <v>0</v>
       </c>
@@ -1009,15 +1103,41 @@
       <c r="F22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="6">
+      <c r="I22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="7">
+        <f>ABS(J21/3)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K22" s="7">
+        <f t="shared" ref="K22" si="1">ABS(K21/4)</f>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="L22" s="7">
+        <f t="shared" ref="L22" si="2">ABS(L21/4)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M22" s="7">
+        <f>ABS(M21/10)</f>
+        <v>0.43</v>
+      </c>
+      <c r="N22" s="7">
+        <f>ABS(N21/10)</f>
+        <v>0.24285714285714283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
+      <c r="C23">
+        <v>-1</v>
+      </c>
       <c r="D23">
         <v>0</v>
       </c>
@@ -1028,14 +1148,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
       <c r="D24">
         <v>0</v>
       </c>
@@ -1046,13 +1169,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B25">
         <v>0</v>
+      </c>
+      <c r="C25">
+        <v>-2</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1064,14 +1190,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
       <c r="D26">
         <v>0</v>
       </c>
@@ -1082,14 +1211,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
+      <c r="C27">
+        <v>-1</v>
+      </c>
       <c r="D27">
         <v>0</v>
       </c>
@@ -1100,13 +1232,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="6">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B28">
         <v>0</v>
+      </c>
+      <c r="C28">
+        <v>-1</v>
       </c>
       <c r="D28">
         <v>-1</v>
@@ -1118,13 +1253,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="6">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B29">
         <v>0</v>
+      </c>
+      <c r="C29">
+        <v>-0.5</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1135,14 +1273,20 @@
       <c r="F29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
+      <c r="G29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B30">
         <v>0</v>
+      </c>
+      <c r="C30">
+        <v>-0.5</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1157,13 +1301,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="6">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B31">
         <v>0</v>
+      </c>
+      <c r="C31">
+        <v>-2</v>
       </c>
       <c r="D31">
         <v>-2</v>
@@ -1175,13 +1322,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B32">
         <v>0</v>
+      </c>
+      <c r="C32">
+        <v>-0.5</v>
       </c>
       <c r="D32">
         <v>-1</v>
@@ -1193,13 +1343,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B33">
         <v>0</v>
+      </c>
+      <c r="C33">
+        <v>-0.5</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1211,14 +1364,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="6">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
       <c r="D34">
         <v>0</v>
       </c>
@@ -1229,13 +1385,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="6">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B35">
         <v>0</v>
+      </c>
+      <c r="C35">
+        <v>-2</v>
       </c>
       <c r="D35">
         <v>-2</v>
@@ -1250,13 +1409,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="6">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B36">
         <v>0</v>
+      </c>
+      <c r="C36">
+        <v>-2</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1268,14 +1430,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="6">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
+      <c r="C37">
+        <v>-0.5</v>
+      </c>
       <c r="D37">
         <v>0</v>
       </c>
@@ -1285,7 +1450,7 @@
       <c r="F37" t="b">
         <v>0</v>
       </c>
-      <c r="I37" s="5" t="s">
+      <c r="I37" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J37">
@@ -1293,26 +1458,33 @@
         <v>0</v>
       </c>
       <c r="K37">
+        <f>COUNTIF(C22:C40,"&lt;&gt;0")</f>
+        <v>15</v>
+      </c>
+      <c r="L37">
         <f>COUNTIF(D22:D40,"&lt;&gt;0")</f>
         <v>5</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <f>COUNTIF(E22:E40,"&lt;&gt;0")</f>
         <v>8</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <f>COUNTIFS(E22:E40,"&lt;&gt;0",F22:F40,"FALSE")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="6">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
+      <c r="C38">
+        <v>-0.5</v>
+      </c>
       <c r="D38">
         <v>0</v>
       </c>
@@ -1322,7 +1494,7 @@
       <c r="F38" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="I38" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J38">
@@ -1330,25 +1502,32 @@
         <v>0</v>
       </c>
       <c r="K38">
+        <f>SUM(C22:C40)</f>
+        <v>-16.5</v>
+      </c>
+      <c r="L38">
         <f>SUM(D22:D40)</f>
         <v>-7</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <f>SUM(E22:E40)</f>
         <v>-20</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <f>SUMIF(F22:F40,"FALSE",E22:E40)</f>
         <v>-10</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="6">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B39">
         <v>0</v>
+      </c>
+      <c r="C39">
+        <v>-0.5</v>
       </c>
       <c r="D39">
         <v>-1</v>
@@ -1359,7 +1538,7 @@
       <c r="F39" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="I39" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J39">
@@ -1367,26 +1546,33 @@
         <v>0</v>
       </c>
       <c r="K39">
+        <f>AVERAGE(C22:C40)</f>
+        <v>-0.86842105263157898</v>
+      </c>
+      <c r="L39">
         <f>AVERAGE(D22:D40)</f>
         <v>-0.36842105263157893</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <f>AVERAGE(E22:E40)</f>
         <v>-1.0526315789473684</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <f>AVERAGEIF(F22:F40,"FALSE",E22:E40)</f>
         <v>-0.55555555555555558</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="6">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
         <f>A39+1</f>
         <v>18</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
+      <c r="C40">
+        <v>-2</v>
+      </c>
       <c r="D40">
         <v>0</v>
       </c>
@@ -1396,60 +1582,94 @@
       <c r="F40" t="b">
         <v>0</v>
       </c>
-      <c r="I40" s="5" t="s">
+      <c r="I40" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J40" t="s">
         <v>21</v>
       </c>
       <c r="K40">
+        <f>AVERAGEIF(C22:C40,"&lt;&gt;0")</f>
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="L40">
         <f>AVERAGEIF(D22:D40,"&lt;&gt;0")</f>
         <v>-1.4</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <f>AVERAGEIF(E22:E40,"&lt;&gt;0")</f>
         <v>-2.5</v>
       </c>
-      <c r="M40">
+      <c r="N40">
         <f>AVERAGEIFS(E22:E40,E22:E40,"&lt;&gt;0",F22:F40,"FALSE")</f>
         <v>-1.4285714285714286</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B41">
         <f>COUNTIF(B2:B40,"&lt;&gt;0")</f>
         <v>3</v>
       </c>
+      <c r="C41">
+        <f>COUNTIF(C2:C40,"&lt;&gt;0")</f>
+        <v>33</v>
+      </c>
       <c r="D41">
-        <f t="shared" ref="D41:E41" si="1">COUNTIF(D2:D40,"&lt;&gt;0")</f>
+        <f t="shared" ref="D41:E41" si="3">COUNTIF(D2:D40,"&lt;&gt;0")</f>
         <v>8</v>
       </c>
       <c r="E41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="F41">
         <f>COUNTIFS(E2:E40,"&lt;&gt;0",F2:F40,"FALSE")</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
+      <c r="I41" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K41" s="7">
+        <f t="shared" ref="K41" si="4">ABS(K40/4)</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="L41" s="7">
+        <f t="shared" ref="L41" si="5">ABS(L40/4)</f>
+        <v>0.35</v>
+      </c>
+      <c r="M41" s="7">
+        <f>ABS(M40/10)</f>
+        <v>0.25</v>
+      </c>
+      <c r="N41" s="7">
+        <f>ABS(N40/10)</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B42">
         <f>SUM(B2:B40)</f>
         <v>-1.5</v>
       </c>
+      <c r="C42">
+        <f>SUM(C2:C40)</f>
+        <v>-44.5</v>
+      </c>
       <c r="D42">
-        <f t="shared" ref="D42:E42" si="2">SUM(D2:D40)</f>
+        <f t="shared" ref="D42:E42" si="6">SUM(D2:D40)</f>
         <v>-9</v>
       </c>
       <c r="E42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-63</v>
       </c>
       <c r="F42">
@@ -1457,20 +1677,24 @@
         <v>-27</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B43">
         <f>AVERAGE(B2:B40)</f>
         <v>-3.8461538461538464E-2</v>
       </c>
+      <c r="C43">
+        <f>AVERAGE(C2:C40)</f>
+        <v>-1.141025641025641</v>
+      </c>
       <c r="D43">
-        <f t="shared" ref="D43:E43" si="3">AVERAGE(D2:D40)</f>
+        <f t="shared" ref="D43:E43" si="7">AVERAGE(D2:D40)</f>
         <v>-0.23076923076923078</v>
       </c>
       <c r="E43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1.6153846153846154</v>
       </c>
       <c r="F43">
@@ -1478,20 +1702,24 @@
         <v>-0.77142857142857146</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B44">
         <f>AVERAGEIF(B2:B40,"&lt;&gt;0")</f>
         <v>-0.5</v>
       </c>
+      <c r="C44">
+        <f>AVERAGEIF(C2:C40,"&lt;&gt;0")</f>
+        <v>-1.3484848484848484</v>
+      </c>
       <c r="D44">
-        <f t="shared" ref="D44:E44" si="4">AVERAGEIF(D2:D40,"&lt;&gt;0")</f>
+        <f t="shared" ref="D44:E44" si="8">AVERAGEIF(D2:D40,"&lt;&gt;0")</f>
         <v>-1.125</v>
       </c>
       <c r="E44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-3.5</v>
       </c>
       <c r="F44">
@@ -1499,10 +1727,35 @@
         <v>-1.9285714285714286</v>
       </c>
     </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="7">
+        <f>ABS(B44/4)</f>
+        <v>0.125</v>
+      </c>
+      <c r="C45" s="7">
+        <f t="shared" ref="C45:D45" si="9">ABS(C44/4)</f>
+        <v>0.3371212121212121</v>
+      </c>
+      <c r="D45" s="7">
+        <f t="shared" si="9"/>
+        <v>0.28125</v>
+      </c>
+      <c r="E45" s="7">
+        <f>ABS(E44/10)</f>
+        <v>0.35</v>
+      </c>
+      <c r="F45" s="7">
+        <f>ABS(F44/10)</f>
+        <v>0.19285714285714287</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="J18:M21 J37:M40" formulaRange="1"/>
+    <ignoredError sqref="L18:N21 L37:N40 J37:J40 J18:J21 K18:K21 K37:K40" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>